<commit_message>
Agrego nuevos quierys al excel
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="eventos(MySQL)" sheetId="4" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="eventos(Cassandra)" sheetId="6" r:id="rId6"/>
     <sheet name="usuarios_has_eventos(Cassandra)" sheetId="7" r:id="rId7"/>
     <sheet name="usuarios_has_eventos(MySQL)" sheetId="8" r:id="rId8"/>
+    <sheet name="grupos_has_usuarios(MySQL)" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="718">
   <si>
     <t>INSERT INTO `grupos` (`idgrupo`,`dsgrupo`) VALUES (91,"Sodales Nisi Magna Ltd"),(92,"Arcu Aliquam LLP"),(93,"Consectetuer LLC"),(94,"Nibh Vulputate Mauris LLP"),(95,"Nonummy Ipsum Non Institute"),(96,"Sociis Natoque Penatibus Inc."),(97,"Eget Institute"),(98,"Nunc Nulla Consulting"),(99,"Sed Pharetra Felis Corporation"),(100,"Nec Ante Foundation");</t>
   </si>
@@ -1875,6 +1876,306 @@
   </si>
   <si>
     <t>INSERT INTO `usuarios_has_eventos` (`usuarios_idusuario`,`eventos_idevento`) VALUES (20,97);</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (26,1,"Y");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (97,2,"Y");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (6,3,"Y");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (22,4,"Y");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (24,5,"Y");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (58,6,"Y");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (80,7,"Y");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (94,8,"Y");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (23,9,"Y");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (7,10,"Y");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (14,11,"Y");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (51,12,"Y");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (9,13,"Y");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (5,14,"Y");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (5,15,"Y");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (21,16,"Y");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (18,17,"Y");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (56,18,"Y");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (96,19,"Y");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (44,20,"Y");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (82,1,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (81,1,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (99,1,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (65,1,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (3,2,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (42,2,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (58,2,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (80,2,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (28,3,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (4,3,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (92,3,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (19,3,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (42,4,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (64,4,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (11,4,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (74,4,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (96,5,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (85,5,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (48,5,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (72,5,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (19,6,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (32,6,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (33,6,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (67,6,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (9,7,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (67,7,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (51,7,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (83,7,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (51,8,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (70,8,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (84,8,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (48,8,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (46,9,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (24,9,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (35,9,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (13,9,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (92,10,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (75,10,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (9,10,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (42,10,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (23,11,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (78,11,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (8,11,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (19,11,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (36,12,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (77,12,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (16,12,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (29,12,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (38,13,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (70,13,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (100,13,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (23,13,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (43,14,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (12,14,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (56,14,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (23,14,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (64,15,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (1,15,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (31,15,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (46,15,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (62,16,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (71,16,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (98,16,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (99,16,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (74,17,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (97,17,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (83,17,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (62,17,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (98,18,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (56,18,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (38,18,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (13,18,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (43,19,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (65,19,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (56,19,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (98,19,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (57,20,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (44,20,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (88,20,"N");</t>
+  </si>
+  <si>
+    <t>INSERT INTO `grupos_has_usuarios` (`grupos_idgrupo`,`usuarios_idusuario`,`principal`) VALUES (79,20,"N");</t>
   </si>
 </sst>
 </file>
@@ -4923,7 +5224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A100"/>
     </sheetView>
   </sheetViews>
@@ -5432,4 +5733,517 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A100"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>717</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>